<commit_message>
exel + kodowanie, dalej mi sie nie chce xddd
</commit_message>
<xml_diff>
--- a/jedzenie.xlsx
+++ b/jedzenie.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$M$3:$M$44</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="125">
   <si>
     <t>składniki</t>
   </si>
@@ -400,10 +405,28 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -481,8 +504,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -496,8 +531,20 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+  <cellStyles count="13">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Standardowy" xfId="0" builtinId="0"/>
+    <cellStyle name="Użyte hiperłącze" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Użyte hiperłącze" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Użyte hiperłącze" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Użyte hiperłącze" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Użyte hiperłącze" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Użyte hiperłącze" xfId="12" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -798,18 +845,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H3:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="M44" sqref="M4:M44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="8" max="9" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="8" max="9" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="8:13">
       <c r="H3" t="s">
         <v>0</v>
       </c>
@@ -817,7 +864,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="8:13">
       <c r="H4" t="s">
         <v>32</v>
       </c>
@@ -825,7 +872,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="8:13">
       <c r="H5" t="s">
         <v>50</v>
       </c>
@@ -836,7 +883,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="8:13">
       <c r="H6" t="s">
         <v>9</v>
       </c>
@@ -844,7 +891,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="8:13">
       <c r="H7" t="s">
         <v>3</v>
       </c>
@@ -855,7 +902,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="8:13">
       <c r="H8" t="s">
         <v>43</v>
       </c>
@@ -863,7 +910,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:13">
       <c r="H9" t="s">
         <v>55</v>
       </c>
@@ -871,7 +918,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:13">
       <c r="H10" t="s">
         <v>44</v>
       </c>
@@ -882,7 +929,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="8:13">
       <c r="H11" t="s">
         <v>1</v>
       </c>
@@ -890,7 +937,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:13">
       <c r="H12" t="s">
         <v>69</v>
       </c>
@@ -898,7 +945,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:13">
       <c r="H13" t="s">
         <v>37</v>
       </c>
@@ -906,7 +953,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="8:13">
       <c r="H14" t="s">
         <v>75</v>
       </c>
@@ -917,7 +964,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="8:13">
       <c r="H15" t="s">
         <v>2</v>
       </c>
@@ -925,7 +972,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="8:13">
       <c r="H16" t="s">
         <v>7</v>
       </c>
@@ -933,7 +980,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:13">
       <c r="H17" t="s">
         <v>17</v>
       </c>
@@ -941,7 +988,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:13">
       <c r="H18" t="s">
         <v>56</v>
       </c>
@@ -949,7 +996,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:13">
       <c r="H19" t="s">
         <v>25</v>
       </c>
@@ -957,7 +1004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:13">
       <c r="H20" t="s">
         <v>14</v>
       </c>
@@ -965,7 +1012,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:13">
       <c r="H21" t="s">
         <v>74</v>
       </c>
@@ -973,7 +1020,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:13">
       <c r="H22" t="s">
         <v>11</v>
       </c>
@@ -981,7 +1028,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:13">
       <c r="H23" t="s">
         <v>20</v>
       </c>
@@ -989,7 +1036,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:13">
       <c r="H24" t="s">
         <v>22</v>
       </c>
@@ -997,7 +1044,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:13">
       <c r="H25" t="s">
         <v>4</v>
       </c>
@@ -1005,7 +1052,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:13">
       <c r="H26" t="s">
         <v>72</v>
       </c>
@@ -1013,7 +1060,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:13">
       <c r="H27" t="s">
         <v>31</v>
       </c>
@@ -1021,7 +1068,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:13">
       <c r="H28" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1076,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:13">
       <c r="H29" t="s">
         <v>66</v>
       </c>
@@ -1037,7 +1084,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:13">
       <c r="H30" t="s">
         <v>53</v>
       </c>
@@ -1045,7 +1092,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:13">
       <c r="H31" t="s">
         <v>10</v>
       </c>
@@ -1053,7 +1100,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:13">
       <c r="H32" t="s">
         <v>62</v>
       </c>
@@ -1061,7 +1108,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:13">
       <c r="H33" t="s">
         <v>21</v>
       </c>
@@ -1069,7 +1116,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:13">
       <c r="H34" t="s">
         <v>6</v>
       </c>
@@ -1077,7 +1124,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:13">
       <c r="H35" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1132,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:13">
       <c r="H36" t="s">
         <v>24</v>
       </c>
@@ -1093,7 +1140,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:13">
       <c r="H37" t="s">
         <v>15</v>
       </c>
@@ -1101,7 +1148,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:13">
       <c r="H38" t="s">
         <v>13</v>
       </c>
@@ -1109,7 +1156,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:13">
       <c r="H39" t="s">
         <v>18</v>
       </c>
@@ -1117,7 +1164,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:13">
       <c r="H40" t="s">
         <v>39</v>
       </c>
@@ -1125,7 +1172,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:13">
       <c r="H41" t="s">
         <v>8</v>
       </c>
@@ -1133,22 +1180,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:13">
       <c r="M42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:13">
       <c r="M43" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:13">
       <c r="M44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:13">
       <c r="L45">
         <v>1</v>
       </c>
@@ -1163,6 +1210,12 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1170,26 +1223,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:BY258"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="116.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="116.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.85546875" customWidth="1"/>
-    <col min="76" max="76" width="14.140625" customWidth="1"/>
-    <col min="78" max="78" width="32.5703125" customWidth="1"/>
+    <col min="29" max="29" width="12.83203125" customWidth="1"/>
+    <col min="76" max="76" width="14.1640625" customWidth="1"/>
+    <col min="78" max="78" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77">
       <c r="H4" s="2" t="s">
         <v>79</v>
       </c>
@@ -1401,7 +1454,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77">
       <c r="H5" t="s">
         <v>32</v>
       </c>
@@ -1613,7 +1666,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -1843,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77">
       <c r="G7" t="str">
         <f>H7&amp;I7&amp;J7&amp;K7&amp;L7&amp;M7&amp;N7&amp;O7&amp;P7&amp;Q7&amp;R7&amp;S7&amp;T7&amp;U7&amp;V7&amp;W7&amp;X7&amp;Y7&amp;Z7&amp;AA7&amp;AB7&amp;AC7&amp;AD7&amp;AE7&amp;AF7&amp;AG7&amp;AH7&amp;AI7&amp;AJ7&amp;AK7&amp;AL7&amp;AM7&amp;AN7&amp;AO7&amp;AP7&amp;AQ7&amp;AR7&amp;AS7&amp;AT7&amp;AU7&amp;AV7&amp;AW7&amp;AY7&amp;AZ7&amp;BA7&amp;BB7&amp;BC7&amp;BD7&amp;BE7&amp;BF7&amp;BG7&amp;BH7&amp;BI7&amp;BJ7&amp;BK7&amp;BL7&amp;BM7&amp;BN7&amp;BO7&amp;BP7&amp;BQ7&amp;BR7&amp;BS7&amp;BT7&amp;BU7&amp;BV7&amp;BW7&amp;BX7&amp;BY7</f>
         <v>attributeContain("skladniki","bagietka")attributeContain("skladniki","olej")attributeContain("skladniki","ziemniaki")attributeContain("pic_jesc","jeść")attributeContain("smak","słony")attributeContain("czas","30 min")attributeContain("czas","60 min")attributeContain("czas","więcej")attributeContain("sprzet","piekarnik")attributeContain("sprzet","patelnia")attributeContain("sprzet","frytkownica")attributeContain("cieplo_zimno","ciepło")attributeContain("zmywanie","tak")attributeContain("glodny","średnio")attributeContain("glodny","bardzo")attributeContain("bogato","tak, na bogato")attributeContain("bogato","bieda")</v>
@@ -2125,7 +2178,7 @@
         <v>attributeContain("bogato","bieda")</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77">
       <c r="F8" t="s">
         <v>123</v>
       </c>
@@ -2393,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77">
       <c r="G9" t="str">
         <f t="shared" si="2"/>
         <v>attributeContain("skladniki","bagietka")attributeContain("skladniki","parówki")attributeContain("pic_jesc","jeść")attributeContain("czas","10 min")attributeContain("czas","30 min")attributeContain("czas","60 min")attributeContain("czas","więcej")attributeContain("sprzet","mikrofalówka")attributeContain("cieplo_zimno","ciepło")attributeContain("wegetarianskie","nie")attributeContain("zmywanie","nie")attributeContain("glodny","lekko")attributeContain("bogato","bieda")</v>
@@ -2675,7 +2728,7 @@
         <v>attributeContain("bogato","bieda")</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77">
       <c r="F10" t="s">
         <v>70</v>
       </c>
@@ -2936,7 +2989,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77">
       <c r="G11" t="str">
         <f t="shared" si="2"/>
         <v>attributeContain("skladniki","cebula")attributeContain("skladniki","kapusta")attributeContain("skladniki","kapusta kiszona")attributeContain("skladniki","kiełbasa")attributeContain("skladniki","mięso ")attributeContain("skladniki","olej")attributeContain("skladniki","szynka")attributeContain("pic_jesc","jeść")attributeContain("smak","kwaśny")attributeContain("czas","60 min")attributeContain("czas","więcej")attributeContain("sprzet","kuchenka")attributeContain("sprzet","garnek")attributeContain("sprzet","patelnia")attributeContain("cieplo_zimno","ciepło")attributeContain("wegetarianskie","nie")attributeContain("zmywanie","tak")attributeContain("glodny","średnio")attributeContain("glodny","bardzo")attributeContain("bogato","tak, na bogato")</v>
@@ -3218,7 +3271,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77">
       <c r="F12" t="s">
         <v>52</v>
       </c>
@@ -3291,7 +3344,7 @@
         <v/>
       </c>
       <c r="X12" t="str">
-        <f t="shared" ref="X12:BY12" si="9">IF(X11=1,CONCATENATE($A$6,X$4,$B$6,X$5,$C$6),"")</f>
+        <f t="shared" ref="X12:BX12" si="9">IF(X11=1,CONCATENATE($A$6,X$4,$B$6,X$5,$C$6),"")</f>
         <v/>
       </c>
       <c r="Y12" t="str">
@@ -3484,7 +3537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77">
       <c r="G13" t="str">
         <f t="shared" si="2"/>
         <v>attributeContain("skladniki","śmietana")attributeContain("skladniki","ziemniaki")attributeContain("pic_jesc","jeść")attributeContain("smak","słony")attributeContain("czas","30 min")attributeContain("czas","60 min")attributeContain("czas","więcej")attributeContain("sprzet","kuchenka")attributeContain("sprzet","garnek")attributeContain("sprzet","patelnia")attributeContain("cieplo_zimno","ciepło")attributeContain("cieplo_zimno","zimno")attributeContain("zmywanie","nie")attributeContain("glodny","lekko")attributeContain("glodny","średnio")attributeContain("glodny","bardzo")attributeContain("bogato","bieda")</v>
@@ -3766,7 +3819,7 @@
         <v>attributeContain("bogato","bieda")</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:77">
       <c r="F14" t="s">
         <v>19</v>
       </c>
@@ -3830,7 +3883,7 @@
         <v>1</v>
       </c>
       <c r="X14" t="str">
-        <f t="shared" ref="X14:BY14" si="11">IF(X13=1,CONCATENATE($A$6,X$4,$B$6,X$5,$C$6),"")</f>
+        <f t="shared" ref="X14:BX14" si="11">IF(X13=1,CONCATENATE($A$6,X$4,$B$6,X$5,$C$6),"")</f>
         <v/>
       </c>
       <c r="Y14">
@@ -4003,7 +4056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:77">
       <c r="G15" t="str">
         <f t="shared" si="2"/>
         <v>attributeContain("skladniki","bagietka")attributeContain("skladniki","bułka")attributeContain("skladniki","cebula")attributeContain("skladniki","chleb")attributeContain("skladniki","dżem")attributeContain("skladniki","jajka")attributeContain("skladniki","kiełbasa")attributeContain("skladniki","masło")attributeContain("skladniki","mięso ")attributeContain("skladniki","miód")attributeContain("skladniki","nutella")attributeContain("skladniki","ogórek")attributeContain("skladniki","papryka")attributeContain("skladniki","parówki")attributeContain("skladniki","pasztet")attributeContain("skladniki","pieczarki ")attributeContain("skladniki","pomidor")attributeContain("skladniki","ser pleśniowy ")attributeContain("skladniki","ser twarogowy ")attributeContain("skladniki","ser żółty ")attributeContain("skladniki","szynka")attributeContain("pic_jesc","jeść")attributeContain("smak","słodki")attributeContain("smak","słony")attributeContain("czas","10 min")attributeContain("czas","30 min")attributeContain("czas","60 min")attributeContain("czas","więcej")attributeContain("glodny","lekko")attributeContain("glodny","średnio")attributeContain("bogato","bieda")</v>
@@ -4285,15 +4338,14 @@
         <v>attributeContain("bogato","bieda")</v>
       </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:77">
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
       <c r="G16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H16" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="I16" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4567,7 +4619,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:77">
       <c r="G17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4849,7 +4901,10 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:77">
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
       <c r="G18" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -5131,7 +5186,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:77">
       <c r="G19" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -5413,7 +5468,10 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:77">
+      <c r="F20" t="s">
+        <v>68</v>
+      </c>
       <c r="G20" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -5695,7 +5753,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:77">
       <c r="G21" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -5977,7 +6035,10 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:77">
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -6259,7 +6320,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:77">
       <c r="G23" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -6541,7 +6602,10 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:77">
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
       <c r="G24" t="str">
         <f>H24&amp;I24&amp;J24&amp;K24&amp;L24&amp;M24&amp;N24&amp;O24&amp;P24&amp;Q24&amp;R24&amp;S24&amp;T24&amp;U24&amp;V24&amp;W24&amp;X24&amp;Y24&amp;Z24&amp;AA24&amp;AB24&amp;AC24&amp;AD24&amp;AE24&amp;AF24&amp;AG24&amp;AH24&amp;AI24&amp;AJ24&amp;AK24&amp;AL24&amp;AM24&amp;AN24&amp;AO24&amp;AP24&amp;AQ24&amp;AR24&amp;AS24&amp;AT24&amp;AU24&amp;AV24&amp;AW24&amp;AY24&amp;AZ24&amp;BA24&amp;BB24&amp;BC24&amp;BD24&amp;BE24&amp;BF24&amp;BG24&amp;BH24&amp;BI24&amp;BJ24&amp;BK24&amp;BL24&amp;BM24&amp;BN24&amp;BO24&amp;BP24&amp;BQ24&amp;BR24&amp;BS24&amp;BT24&amp;BU24&amp;BV24&amp;BW24&amp;BX24&amp;BY24</f>
         <v/>
@@ -6823,7 +6887,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:77">
       <c r="G25" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -7105,7 +7169,10 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:77">
+      <c r="F26" t="s">
+        <v>48</v>
+      </c>
       <c r="G26" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -7383,7 +7450,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:77">
       <c r="G27" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -7661,7 +7728,10 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:77">
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
       <c r="G28" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -7939,7 +8009,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:77">
       <c r="G29" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8217,7 +8287,10 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:77">
+      <c r="F30" t="s">
+        <v>36</v>
+      </c>
       <c r="G30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8495,7 +8568,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:77">
       <c r="G31" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8773,7 +8846,10 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:77">
+      <c r="F32" t="s">
+        <v>76</v>
+      </c>
       <c r="G32" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9051,7 +9127,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:77">
       <c r="G33" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9329,7 +9405,10 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:77">
+      <c r="F34" t="s">
+        <v>47</v>
+      </c>
       <c r="G34" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9607,7 +9686,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:77">
       <c r="G35" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9885,7 +9964,10 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:77">
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
       <c r="G36" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -10163,7 +10245,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:77">
       <c r="G37" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -10441,7 +10523,10 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:77">
+      <c r="F38" t="s">
+        <v>49</v>
+      </c>
       <c r="G38" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -10719,7 +10804,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:77">
       <c r="G39" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -10997,7 +11082,10 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:77">
+      <c r="F40" t="s">
+        <v>64</v>
+      </c>
       <c r="G40" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -11275,7 +11363,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:77">
       <c r="G41" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -11553,7 +11641,10 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:77">
+      <c r="F42" t="s">
+        <v>35</v>
+      </c>
       <c r="G42" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -11831,7 +11922,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:77">
       <c r="G43" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12109,7 +12200,10 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:77">
+      <c r="F44" t="s">
+        <v>27</v>
+      </c>
       <c r="G44" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12387,7 +12481,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:77">
       <c r="G45" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12665,7 +12759,10 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:77">
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
       <c r="G46" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12943,7 +13040,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:77">
       <c r="G47" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13221,7 +13318,10 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:77">
+      <c r="F48" t="s">
+        <v>67</v>
+      </c>
       <c r="G48" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13499,7 +13599,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:77">
       <c r="G49" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13777,7 +13877,10 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:77">
+      <c r="F50" t="s">
+        <v>71</v>
+      </c>
       <c r="G50" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -14055,7 +14158,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:77">
       <c r="G51" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -14333,7 +14436,10 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:77">
+      <c r="F52" t="s">
+        <v>73</v>
+      </c>
       <c r="G52" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -14611,7 +14717,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:77">
       <c r="G53" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -14889,7 +14995,10 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:77">
+      <c r="F54" t="s">
+        <v>33</v>
+      </c>
       <c r="G54" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -15163,7 +15272,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:77">
       <c r="G55" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -15437,7 +15546,10 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:77">
+      <c r="F56" t="s">
+        <v>34</v>
+      </c>
       <c r="G56" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -15711,7 +15823,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:77">
       <c r="G57" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -15985,7 +16097,10 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:77">
+      <c r="F58" t="s">
+        <v>28</v>
+      </c>
       <c r="G58" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -16259,7 +16374,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:77">
       <c r="G59" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -16533,7 +16648,10 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:77">
+      <c r="F60" t="s">
+        <v>77</v>
+      </c>
       <c r="G60" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -16807,7 +16925,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:77">
       <c r="G61" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -17081,7 +17199,10 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:77">
+      <c r="F62" t="s">
+        <v>40</v>
+      </c>
       <c r="G62" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -17355,7 +17476,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:77">
       <c r="G63" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -17629,7 +17750,10 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:77">
+      <c r="F64" t="s">
+        <v>11</v>
+      </c>
       <c r="G64" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -17903,7 +18027,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:77">
       <c r="G65" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -18177,7 +18301,10 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:77">
+      <c r="F66" t="s">
+        <v>54</v>
+      </c>
       <c r="G66" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -18451,7 +18578,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:77">
       <c r="G67" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -18725,7 +18852,10 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:77">
+      <c r="F68" t="s">
+        <v>57</v>
+      </c>
       <c r="G68" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -18999,7 +19129,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:77">
       <c r="G69" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -19273,7 +19403,10 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:77">
+      <c r="F70" t="s">
+        <v>42</v>
+      </c>
       <c r="G70" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -19547,7 +19680,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:77">
       <c r="G71" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -19821,7 +19954,10 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:77">
+      <c r="F72" t="s">
+        <v>63</v>
+      </c>
       <c r="G72" t="str">
         <f t="shared" ref="G72:G128" si="72">H72&amp;I72&amp;J72&amp;K72&amp;L72&amp;M72&amp;N72&amp;O72&amp;P72&amp;Q72&amp;R72&amp;S72&amp;T72&amp;U72&amp;V72&amp;W72&amp;X72&amp;Y72&amp;Z72&amp;AA72&amp;AB72&amp;AC72&amp;AD72&amp;AE72&amp;AF72&amp;AG72&amp;AH72&amp;AI72&amp;AJ72&amp;AK72&amp;AL72&amp;AM72&amp;AN72&amp;AO72&amp;AP72&amp;AQ72&amp;AR72&amp;AS72&amp;AT72&amp;AU72&amp;AV72&amp;AW72&amp;AY72&amp;AZ72&amp;BA72&amp;BB72&amp;BC72&amp;BD72&amp;BE72&amp;BF72&amp;BG72&amp;BH72&amp;BI72&amp;BJ72&amp;BK72&amp;BL72&amp;BM72&amp;BN72&amp;BO72&amp;BP72&amp;BQ72&amp;BR72&amp;BS72&amp;BT72&amp;BU72&amp;BV72&amp;BW72&amp;BX72&amp;BY72</f>
         <v/>
@@ -20095,7 +20231,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:77">
       <c r="G73" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -20369,7 +20505,10 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:77">
+      <c r="F74" t="s">
+        <v>58</v>
+      </c>
       <c r="G74" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -20643,7 +20782,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:77">
       <c r="G75" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -20917,7 +21056,10 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:77">
+      <c r="F76" t="s">
+        <v>53</v>
+      </c>
       <c r="G76" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -21191,7 +21333,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:77">
       <c r="G77" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -21465,7 +21607,10 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="78" spans="6:77">
+      <c r="F78" t="s">
+        <v>61</v>
+      </c>
       <c r="G78" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -21739,7 +21884,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:77">
       <c r="G79" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -22013,7 +22158,10 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:77">
+      <c r="F80" t="s">
+        <v>38</v>
+      </c>
       <c r="G80" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -22287,7 +22435,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:77">
       <c r="G81" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -22561,7 +22709,10 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:77">
+      <c r="F82" t="s">
+        <v>12</v>
+      </c>
       <c r="G82" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -22835,7 +22986,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:77">
       <c r="G83" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -23109,7 +23260,10 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:77">
+      <c r="F84" t="s">
+        <v>41</v>
+      </c>
       <c r="G84" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -23383,7 +23537,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:77">
       <c r="G85" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -23657,7 +23811,10 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:77">
+      <c r="F86" t="s">
+        <v>60</v>
+      </c>
       <c r="G86" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -23931,7 +24088,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:77">
       <c r="G87" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -24205,7 +24362,10 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:77">
+      <c r="F88" t="s">
+        <v>30</v>
+      </c>
       <c r="G88" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -24483,7 +24643,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:77">
       <c r="G89" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -24761,7 +24921,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:77">
       <c r="G90" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -25039,7 +25199,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:77">
       <c r="G91" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -25317,7 +25477,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:77">
       <c r="G92" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -25595,7 +25755,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:77">
       <c r="G93" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -25873,7 +26033,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:77">
       <c r="G94" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -26151,7 +26311,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:77">
       <c r="G95" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -26429,7 +26589,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:77">
       <c r="G96" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -26707,7 +26867,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:77">
       <c r="G97" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -26985,7 +27145,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:77">
       <c r="G98" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -27263,7 +27423,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:77">
       <c r="G99" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -27541,7 +27701,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:77">
       <c r="G100" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -27819,7 +27979,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:77">
       <c r="G101" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -28097,7 +28257,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:77">
       <c r="G102" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -28375,7 +28535,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:77">
       <c r="G103" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -28653,7 +28813,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="104" spans="7:77">
       <c r="G104" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -28931,7 +29091,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="105" spans="7:77">
       <c r="G105" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -29209,7 +29369,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="106" spans="7:77">
       <c r="G106" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -29487,7 +29647,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:77">
       <c r="G107" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -29765,7 +29925,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:77">
       <c r="G108" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -30043,7 +30203,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="109" spans="7:77">
       <c r="G109" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -30321,7 +30481,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="110" spans="7:77">
       <c r="G110" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -30599,7 +30759,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="111" spans="7:77">
       <c r="G111" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -30877,7 +31037,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="112" spans="7:77">
       <c r="G112" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -31155,7 +31315,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="113" spans="7:77">
       <c r="G113" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -31433,7 +31593,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="114" spans="7:77">
       <c r="G114" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -31711,7 +31871,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="115" spans="7:77">
       <c r="G115" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -31989,7 +32149,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="116" spans="7:77">
       <c r="G116" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -32267,7 +32427,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="117" spans="7:77">
       <c r="G117" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -32545,7 +32705,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="118" spans="7:77">
       <c r="G118" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -32823,7 +32983,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="119" spans="7:77">
       <c r="G119" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -33101,7 +33261,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="120" spans="7:77">
       <c r="G120" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -33379,7 +33539,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="121" spans="7:77">
       <c r="G121" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -33657,7 +33817,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="122" spans="7:77">
       <c r="G122" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -33935,7 +34095,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="123" spans="7:77">
       <c r="G123" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -34213,7 +34373,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="124" spans="7:77">
       <c r="G124" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -34491,7 +34651,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="125" spans="7:77">
       <c r="G125" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -34769,7 +34929,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="126" spans="7:77">
       <c r="G126" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -35047,7 +35207,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="127" spans="7:77">
       <c r="G127" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -35325,7 +35485,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="7:77" x14ac:dyDescent="0.25">
+    <row r="128" spans="7:77">
       <c r="G128" t="str">
         <f t="shared" si="72"/>
         <v/>
@@ -35603,7 +35763,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:77">
       <c r="H129" t="str">
         <f t="shared" si="124"/>
         <v/>
@@ -35877,7 +36037,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:77">
       <c r="H130" t="str">
         <f t="shared" si="124"/>
         <v/>
@@ -36151,7 +36311,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:77">
       <c r="H131" t="str">
         <f t="shared" si="124"/>
         <v/>
@@ -36425,7 +36585,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:77">
       <c r="H132" t="str">
         <f t="shared" si="124"/>
         <v/>
@@ -36699,7 +36859,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:77">
       <c r="H133" t="str">
         <f t="shared" si="124"/>
         <v/>
@@ -36973,7 +37133,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="134" spans="8:77">
       <c r="H134" t="str">
         <f t="shared" si="124"/>
         <v/>
@@ -37247,7 +37407,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="135" spans="8:77">
       <c r="H135" t="str">
         <f t="shared" si="124"/>
         <v/>
@@ -37521,7 +37681,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="136" spans="8:77">
       <c r="H136" t="str">
         <f t="shared" ref="H136:W151" si="141">IF(H135=1,CONCATENATE($A$6,H$4,$B$6,H$5,$C$6),"")</f>
         <v/>
@@ -37795,7 +37955,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="137" spans="8:77">
       <c r="H137" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -38069,7 +38229,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="138" spans="8:77">
       <c r="H138" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -38343,7 +38503,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="139" spans="8:77">
       <c r="H139" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -38617,7 +38777,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="140" spans="8:77">
       <c r="H140" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -38891,7 +39051,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="141" spans="8:77">
       <c r="H141" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -39165,7 +39325,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="142" spans="8:77">
       <c r="H142" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -39439,7 +39599,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="143" spans="8:77">
       <c r="H143" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -39713,7 +39873,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="144" spans="8:77">
       <c r="H144" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -39987,7 +40147,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="145" spans="8:77">
       <c r="H145" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -40261,7 +40421,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="146" spans="8:77">
       <c r="H146" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -40535,7 +40695,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="147" spans="8:77">
       <c r="H147" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -40809,7 +40969,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="148" spans="8:77">
       <c r="H148" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -41083,7 +41243,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="149" spans="8:77">
       <c r="H149" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -41357,7 +41517,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="150" spans="8:77">
       <c r="H150" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -41631,7 +41791,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="151" spans="8:77">
       <c r="H151" t="str">
         <f t="shared" si="141"/>
         <v/>
@@ -41905,7 +42065,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="152" spans="8:77">
       <c r="H152" t="str">
         <f t="shared" ref="H152:W167" si="158">IF(H151=1,CONCATENATE($A$6,H$4,$B$6,H$5,$C$6),"")</f>
         <v/>
@@ -42179,7 +42339,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="153" spans="8:77">
       <c r="H153" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -42453,7 +42613,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="154" spans="8:77">
       <c r="H154" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -42727,7 +42887,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="155" spans="8:77">
       <c r="H155" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -43001,7 +43161,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="156" spans="8:77">
       <c r="H156" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -43275,7 +43435,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="157" spans="8:77">
       <c r="H157" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -43549,7 +43709,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="158" spans="8:77">
       <c r="H158" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -43827,7 +43987,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="159" spans="8:77">
       <c r="H159" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -44105,7 +44265,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="160" spans="8:77">
       <c r="H160" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -44383,7 +44543,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="161" spans="8:77">
       <c r="H161" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -44661,7 +44821,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="162" spans="8:77">
       <c r="H162" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -44939,7 +45099,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="163" spans="8:77">
       <c r="H163" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -45217,7 +45377,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="164" spans="8:77">
       <c r="H164" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -45495,7 +45655,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="165" spans="8:77">
       <c r="H165" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -45773,7 +45933,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="166" spans="8:77">
       <c r="H166" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -46051,7 +46211,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="167" spans="8:77">
       <c r="H167" t="str">
         <f t="shared" si="158"/>
         <v/>
@@ -46329,7 +46489,7 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="168" spans="8:77">
       <c r="H168" t="str">
         <f t="shared" ref="H168:W183" si="175">IF(H167=1,CONCATENATE($A$6,H$4,$B$6,H$5,$C$6),"")</f>
         <v/>
@@ -46607,7 +46767,7 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="169" spans="8:77">
       <c r="H169" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -46885,7 +47045,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="170" spans="8:77">
       <c r="H170" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -47163,7 +47323,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="171" spans="8:77">
       <c r="H171" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -47441,7 +47601,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="172" spans="8:77">
       <c r="H172" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -47719,7 +47879,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="173" spans="8:77">
       <c r="H173" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -47997,7 +48157,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="174" spans="8:77">
       <c r="H174" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -48275,7 +48435,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="175" spans="8:77">
       <c r="H175" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -48553,7 +48713,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="176" spans="8:77">
       <c r="H176" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -48831,7 +48991,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="177" spans="8:77">
       <c r="H177" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -49109,7 +49269,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="178" spans="8:77">
       <c r="H178" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -49387,7 +49547,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="179" spans="8:77">
       <c r="H179" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -49665,7 +49825,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="180" spans="8:77">
       <c r="H180" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -49943,7 +50103,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="181" spans="8:77">
       <c r="H181" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -50221,7 +50381,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="182" spans="8:77">
       <c r="H182" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -50499,7 +50659,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="183" spans="8:77">
       <c r="H183" t="str">
         <f t="shared" si="175"/>
         <v/>
@@ -50777,7 +50937,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="184" spans="8:77">
       <c r="H184" t="str">
         <f t="shared" ref="H184:W199" si="192">IF(H183=1,CONCATENATE($A$6,H$4,$B$6,H$5,$C$6),"")</f>
         <v/>
@@ -51055,7 +51215,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="185" spans="8:77">
       <c r="H185" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -51333,7 +51493,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="186" spans="8:77">
       <c r="H186" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -51611,7 +51771,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="187" spans="8:77">
       <c r="H187" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -51889,7 +52049,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="188" spans="8:77">
       <c r="H188" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -52167,7 +52327,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="189" spans="8:77">
       <c r="H189" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -52445,7 +52605,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="190" spans="8:77">
       <c r="H190" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -52723,7 +52883,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="191" spans="8:77">
       <c r="H191" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -53001,7 +53161,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="192" spans="8:77">
       <c r="H192" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -53279,7 +53439,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="193" spans="8:77">
       <c r="H193" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -53557,7 +53717,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="194" spans="8:77">
       <c r="H194" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -53835,7 +53995,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="195" spans="8:77">
       <c r="H195" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -54113,7 +54273,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="196" spans="8:77">
       <c r="H196" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -54391,7 +54551,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="197" spans="8:77">
       <c r="H197" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -54669,7 +54829,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="198" spans="8:77">
       <c r="H198" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -54947,7 +55107,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="199" spans="8:77">
       <c r="H199" t="str">
         <f t="shared" si="192"/>
         <v/>
@@ -55225,7 +55385,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="200" spans="8:77">
       <c r="H200" t="str">
         <f t="shared" ref="H200:W215" si="209">IF(H199=1,CONCATENATE($A$6,H$4,$B$6,H$5,$C$6),"")</f>
         <v/>
@@ -55503,7 +55663,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="201" spans="8:77">
       <c r="H201" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -55781,7 +55941,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="202" spans="8:77">
       <c r="H202" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -56059,7 +56219,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="203" spans="8:77">
       <c r="H203" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -56337,7 +56497,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="204" spans="8:77">
       <c r="H204" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -56615,7 +56775,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="205" spans="8:77">
       <c r="H205" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -56893,7 +57053,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="206" spans="8:77">
       <c r="H206" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -57171,7 +57331,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="207" spans="8:77">
       <c r="H207" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -57449,7 +57609,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="208" spans="8:77">
       <c r="H208" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -57727,7 +57887,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="209" spans="8:77">
       <c r="H209" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -58005,7 +58165,7 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="210" spans="8:77">
       <c r="H210" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -58283,7 +58443,7 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="211" spans="8:77">
       <c r="H211" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -58561,7 +58721,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="212" spans="8:77">
       <c r="H212" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -58839,7 +58999,7 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="213" spans="8:77">
       <c r="H213" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -59117,7 +59277,7 @@
         <v/>
       </c>
     </row>
-    <row r="214" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="214" spans="8:77">
       <c r="H214" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -59395,7 +59555,7 @@
         <v/>
       </c>
     </row>
-    <row r="215" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="215" spans="8:77">
       <c r="H215" t="str">
         <f t="shared" si="209"/>
         <v/>
@@ -59673,7 +59833,7 @@
         <v/>
       </c>
     </row>
-    <row r="216" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="216" spans="8:77">
       <c r="H216" t="str">
         <f t="shared" ref="H216:W231" si="226">IF(H215=1,CONCATENATE($A$6,H$4,$B$6,H$5,$C$6),"")</f>
         <v/>
@@ -59951,7 +60111,7 @@
         <v/>
       </c>
     </row>
-    <row r="217" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="217" spans="8:77">
       <c r="H217" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -60229,7 +60389,7 @@
         <v/>
       </c>
     </row>
-    <row r="218" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="218" spans="8:77">
       <c r="H218" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -60507,7 +60667,7 @@
         <v/>
       </c>
     </row>
-    <row r="219" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="219" spans="8:77">
       <c r="H219" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -60785,7 +60945,7 @@
         <v/>
       </c>
     </row>
-    <row r="220" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="220" spans="8:77">
       <c r="H220" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -61063,7 +61223,7 @@
         <v/>
       </c>
     </row>
-    <row r="221" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="221" spans="8:77">
       <c r="H221" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -61341,7 +61501,7 @@
         <v/>
       </c>
     </row>
-    <row r="222" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="222" spans="8:77">
       <c r="H222" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -61619,7 +61779,7 @@
         <v/>
       </c>
     </row>
-    <row r="223" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="223" spans="8:77">
       <c r="H223" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -61897,7 +62057,7 @@
         <v/>
       </c>
     </row>
-    <row r="224" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="224" spans="8:77">
       <c r="H224" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -62175,7 +62335,7 @@
         <v/>
       </c>
     </row>
-    <row r="225" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="225" spans="8:77">
       <c r="H225" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -62453,7 +62613,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="226" spans="8:77">
       <c r="H226" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -62731,7 +62891,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="227" spans="8:77">
       <c r="H227" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -63009,7 +63169,7 @@
         <v/>
       </c>
     </row>
-    <row r="228" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="228" spans="8:77">
       <c r="H228" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -63287,7 +63447,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="229" spans="8:77">
       <c r="H229" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -63565,7 +63725,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="230" spans="8:77">
       <c r="H230" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -63843,7 +64003,7 @@
         <v/>
       </c>
     </row>
-    <row r="231" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="231" spans="8:77">
       <c r="H231" t="str">
         <f t="shared" si="226"/>
         <v/>
@@ -64121,7 +64281,7 @@
         <v/>
       </c>
     </row>
-    <row r="232" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="232" spans="8:77">
       <c r="H232" t="str">
         <f t="shared" ref="H232:W247" si="243">IF(H231=1,CONCATENATE($A$6,H$4,$B$6,H$5,$C$6),"")</f>
         <v/>
@@ -64399,7 +64559,7 @@
         <v/>
       </c>
     </row>
-    <row r="233" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="233" spans="8:77">
       <c r="H233" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -64677,7 +64837,7 @@
         <v/>
       </c>
     </row>
-    <row r="234" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="234" spans="8:77">
       <c r="H234" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -64955,7 +65115,7 @@
         <v/>
       </c>
     </row>
-    <row r="235" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="235" spans="8:77">
       <c r="H235" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -65233,7 +65393,7 @@
         <v/>
       </c>
     </row>
-    <row r="236" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="236" spans="8:77">
       <c r="H236" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -65511,7 +65671,7 @@
         <v/>
       </c>
     </row>
-    <row r="237" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="237" spans="8:77">
       <c r="H237" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -65789,7 +65949,7 @@
         <v/>
       </c>
     </row>
-    <row r="238" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="238" spans="8:77">
       <c r="H238" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -66067,7 +66227,7 @@
         <v/>
       </c>
     </row>
-    <row r="239" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="239" spans="8:77">
       <c r="H239" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -66345,7 +66505,7 @@
         <v/>
       </c>
     </row>
-    <row r="240" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="240" spans="8:77">
       <c r="H240" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -66623,7 +66783,7 @@
         <v/>
       </c>
     </row>
-    <row r="241" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="241" spans="8:77">
       <c r="H241" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -66901,7 +67061,7 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="242" spans="8:77">
       <c r="H242" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -67179,7 +67339,7 @@
         <v/>
       </c>
     </row>
-    <row r="243" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="243" spans="8:77">
       <c r="H243" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -67457,7 +67617,7 @@
         <v/>
       </c>
     </row>
-    <row r="244" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="244" spans="8:77">
       <c r="H244" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -67735,7 +67895,7 @@
         <v/>
       </c>
     </row>
-    <row r="245" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="245" spans="8:77">
       <c r="H245" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -68013,7 +68173,7 @@
         <v/>
       </c>
     </row>
-    <row r="246" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="246" spans="8:77">
       <c r="H246" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -68291,7 +68451,7 @@
         <v/>
       </c>
     </row>
-    <row r="247" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="247" spans="8:77">
       <c r="H247" t="str">
         <f t="shared" si="243"/>
         <v/>
@@ -68569,7 +68729,7 @@
         <v/>
       </c>
     </row>
-    <row r="248" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="248" spans="8:77">
       <c r="H248" t="str">
         <f t="shared" ref="H248:W258" si="260">IF(H247=1,CONCATENATE($A$6,H$4,$B$6,H$5,$C$6),"")</f>
         <v/>
@@ -68847,7 +69007,7 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="249" spans="8:77">
       <c r="H249" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -69125,7 +69285,7 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="250" spans="8:77">
       <c r="H250" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -69403,7 +69563,7 @@
         <v/>
       </c>
     </row>
-    <row r="251" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="251" spans="8:77">
       <c r="H251" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -69681,7 +69841,7 @@
         <v/>
       </c>
     </row>
-    <row r="252" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="252" spans="8:77">
       <c r="H252" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -69959,7 +70119,7 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="253" spans="8:77">
       <c r="H253" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -70237,7 +70397,7 @@
         <v/>
       </c>
     </row>
-    <row r="254" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="254" spans="8:77">
       <c r="H254" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -70515,7 +70675,7 @@
         <v/>
       </c>
     </row>
-    <row r="255" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="255" spans="8:77">
       <c r="H255" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -70793,7 +70953,7 @@
         <v/>
       </c>
     </row>
-    <row r="256" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="256" spans="8:77">
       <c r="H256" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -71071,7 +71231,7 @@
         <v/>
       </c>
     </row>
-    <row r="257" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="257" spans="8:77">
       <c r="H257" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -71349,7 +71509,7 @@
         <v/>
       </c>
     </row>
-    <row r="258" spans="8:77" x14ac:dyDescent="0.25">
+    <row r="258" spans="8:77">
       <c r="H258" t="str">
         <f t="shared" si="260"/>
         <v/>
@@ -71629,7 +71789,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -71639,8 +71804,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dem jajka i elo
</commit_message>
<xml_diff>
--- a/jedzenie.xlsx
+++ b/jedzenie.xlsx
@@ -504,8 +504,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -549,7 +553,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperłącze" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperłącze" xfId="5" builtinId="8" hidden="1"/>
@@ -565,6 +569,8 @@
     <cellStyle name="Hiperłącze" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperłącze" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperłącze" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Standardowy" xfId="0" builtinId="0"/>
     <cellStyle name="Użyte hiperłącze" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Użyte hiperłącze" xfId="4" builtinId="9" hidden="1"/>
@@ -581,6 +587,8 @@
     <cellStyle name="Użyte hiperłącze" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Użyte hiperłącze" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Użyte hiperłącze" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Użyte hiperłącze" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Użyte hiperłącze" xfId="34" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1259,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:BY258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7652,7 +7660,7 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>111111111111</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="21"/>
@@ -7682,9 +7690,8 @@
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="O28" t="str">
-        <f t="shared" si="21"/>
-        <v/>
+      <c r="O28">
+        <v>1</v>
       </c>
       <c r="P28" t="str">
         <f t="shared" si="21"/>
@@ -7810,17 +7817,15 @@
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="AU28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="AU28">
+        <v>1</v>
       </c>
       <c r="AV28" t="str">
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="AW28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="AW28">
+        <v>1</v>
       </c>
       <c r="AY28" t="str">
         <f t="shared" si="26"/>
@@ -7834,21 +7839,14 @@
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="BB28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="BC28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="BD28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="BE28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="BC28">
+        <v>1</v>
+      </c>
+      <c r="BD28">
+        <v>1</v>
+      </c>
+      <c r="BE28">
+        <v>1</v>
       </c>
       <c r="BF28" t="str">
         <f t="shared" si="26"/>
@@ -7866,9 +7864,8 @@
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="BJ28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="BJ28">
+        <v>1</v>
       </c>
       <c r="BK28" t="str">
         <f t="shared" si="26"/>
@@ -7886,33 +7883,29 @@
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="BO28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="BO28">
+        <v>1</v>
       </c>
       <c r="BP28" t="str">
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="BR28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="BR28">
+        <v>1</v>
       </c>
       <c r="BS28" t="str">
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="BT28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="BT28">
+        <v>1</v>
       </c>
       <c r="BU28" t="str">
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="BV28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="BV28">
+        <v>1</v>
       </c>
       <c r="BW28" t="str">
         <f t="shared" si="26"/>
@@ -7922,15 +7915,14 @@
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="BY28" t="str">
-        <f t="shared" si="26"/>
-        <v/>
+      <c r="BY28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="6:77">
       <c r="G29" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>attributeContain("skladniki","jajka")attributeContain("pic_jesc","jeść")attributeContain("smak","słony")attributeContain("czas","30 min")attributeContain("czas","60 min")attributeContain("czas","więcej")attributeContain("sprzet","garnek")attributeContain("cieplo_zimno","ciepło")attributeContain("wegetarianskie","nie")attributeContain("zmywanie","nie")attributeContain("glodny","średnio")attributeContain("bogato","bieda")</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="21"/>
@@ -7962,7 +7954,7 @@
       </c>
       <c r="O29" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>attributeContain("skladniki","jajka")</v>
       </c>
       <c r="P29" t="str">
         <f t="shared" si="21"/>
@@ -8090,7 +8082,7 @@
       </c>
       <c r="AU29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("pic_jesc","jeść")</v>
       </c>
       <c r="AV29" t="str">
         <f t="shared" si="27"/>
@@ -8098,7 +8090,7 @@
       </c>
       <c r="AW29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("smak","słony")</v>
       </c>
       <c r="AY29" t="str">
         <f t="shared" si="27"/>
@@ -8118,15 +8110,15 @@
       </c>
       <c r="BC29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("czas","30 min")</v>
       </c>
       <c r="BD29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("czas","60 min")</v>
       </c>
       <c r="BE29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("czas","więcej")</v>
       </c>
       <c r="BF29" t="str">
         <f t="shared" si="27"/>
@@ -8146,7 +8138,7 @@
       </c>
       <c r="BJ29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("sprzet","garnek")</v>
       </c>
       <c r="BK29" t="str">
         <f t="shared" si="27"/>
@@ -8166,7 +8158,7 @@
       </c>
       <c r="BO29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("cieplo_zimno","ciepło")</v>
       </c>
       <c r="BP29" t="str">
         <f t="shared" si="27"/>
@@ -8174,7 +8166,7 @@
       </c>
       <c r="BR29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("wegetarianskie","nie")</v>
       </c>
       <c r="BS29" t="str">
         <f t="shared" si="27"/>
@@ -8182,7 +8174,7 @@
       </c>
       <c r="BT29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("zmywanie","nie")</v>
       </c>
       <c r="BU29" t="str">
         <f t="shared" si="27"/>
@@ -8190,7 +8182,7 @@
       </c>
       <c r="BV29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("glodny","średnio")</v>
       </c>
       <c r="BW29" t="str">
         <f t="shared" si="27"/>
@@ -8202,7 +8194,7 @@
       </c>
       <c r="BY29" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>attributeContain("bogato","bieda")</v>
       </c>
     </row>
     <row r="30" spans="6:77">

</xml_diff>